<commit_message>
Add standardized and cleaned data template for cw T2 and update cw T1 crpped excel file
</commit_message>
<xml_diff>
--- a/data/preprocessed/data_standardization_for_nascreening_analysis/mibirem_template/cw_T1_croped_nascreening_mibirem_template - Copy.xlsx
+++ b/data/preprocessed/data_standardization_for_nascreening_analysis/mibirem_template/cw_T1_croped_nascreening_mibirem_template - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aseye001\Sona_Phd\MIBIREM\MiBiPreT_FieldSites\constructed-wetland\data\preprocessed\data_standardization_for_nascreening_analysis\mibirem_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E3A48C-CD7F-4AD8-AFC7-F448D26FA99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703FAB0F-08C4-4BD1-AB6D-F4ABD474731E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chemical analysis" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="214">
   <si>
     <t>Coding</t>
   </si>
@@ -331,72 +331,6 @@
   </si>
   <si>
     <t>Iron II</t>
-  </si>
-  <si>
-    <t>NL_CW_W_01</t>
-  </si>
-  <si>
-    <t>NL_CW_W_02</t>
-  </si>
-  <si>
-    <t>NL_CW_W_03</t>
-  </si>
-  <si>
-    <t>NL_CW_W_04</t>
-  </si>
-  <si>
-    <t>NL_CW_W_05</t>
-  </si>
-  <si>
-    <t>NL_CW_W_06</t>
-  </si>
-  <si>
-    <t>NL_CW_W_07</t>
-  </si>
-  <si>
-    <t>NL_CW_W_08</t>
-  </si>
-  <si>
-    <t>NL_CW_W_09</t>
-  </si>
-  <si>
-    <t>NL_CW_W_010</t>
-  </si>
-  <si>
-    <t>NL_CW_W_011</t>
-  </si>
-  <si>
-    <t>NL_CW_W_012</t>
-  </si>
-  <si>
-    <t>NL_CW_W_013</t>
-  </si>
-  <si>
-    <t>NL_CW_W_014</t>
-  </si>
-  <si>
-    <t>NL_CW_W_015</t>
-  </si>
-  <si>
-    <t>NL_CW_W_016</t>
-  </si>
-  <si>
-    <t>NL_CW_W_017</t>
-  </si>
-  <si>
-    <t>NL_CW_W_018</t>
-  </si>
-  <si>
-    <t>NL_CW_W_019</t>
-  </si>
-  <si>
-    <t>NL_CW_W_020</t>
-  </si>
-  <si>
-    <t>NL_CW_W_021</t>
-  </si>
-  <si>
-    <t>NL_CW_W_022</t>
   </si>
   <si>
     <t>Manganese II</t>
@@ -1062,8 +996,8 @@
   </sheetPr>
   <dimension ref="A1:AV28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1094,28 +1028,28 @@
         <v>98</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>13</v>
@@ -1124,16 +1058,16 @@
         <v>97</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>96</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -1253,22 +1187,22 @@
     </row>
     <row r="3" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>45</v>
@@ -1277,7 +1211,7 @@
         <v>21</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>75</v>
@@ -1306,13 +1240,13 @@
     </row>
     <row r="4" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>74</v>
@@ -1330,10 +1264,10 @@
         <v>71</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>27</v>
@@ -1359,22 +1293,22 @@
     </row>
     <row r="5" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>79</v>
@@ -1383,10 +1317,10 @@
         <v>71</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>58</v>
@@ -1412,16 +1346,16 @@
     </row>
     <row r="6" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>55</v>
@@ -1430,16 +1364,16 @@
         <v>37</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>63</v>
       </c>
       <c r="I6" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>200</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>222</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>63</v>
@@ -1465,19 +1399,19 @@
     </row>
     <row r="7" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>20</v>
@@ -1486,19 +1420,19 @@
         <v>72</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>65</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
       <c r="M7" s="7" t="s">
         <v>32</v>
@@ -1513,24 +1447,24 @@
         <v>34</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>15</v>
@@ -1571,37 +1505,37 @@
     </row>
     <row r="9" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>218</v>
-      </c>
       <c r="K9" s="7" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
       <c r="L9" s="7" t="s">
         <v>92</v>
@@ -1624,10 +1558,10 @@
     </row>
     <row r="10" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>70</v>
@@ -1636,19 +1570,19 @@
         <v>90</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>54</v>
@@ -1677,7 +1611,7 @@
     </row>
     <row r="11" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>14</v>
@@ -1686,16 +1620,16 @@
         <v>19</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>52</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>59</v>
@@ -1707,7 +1641,7 @@
         <v>19</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
       <c r="L11" s="7" t="s">
         <v>83</v>
@@ -1730,10 +1664,10 @@
     </row>
     <row r="12" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>86</v>
@@ -1751,13 +1685,13 @@
         <v>62</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>80</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>85</v>
@@ -1783,10 +1717,10 @@
     </row>
     <row r="13" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>25</v>
@@ -1795,7 +1729,7 @@
         <v>36</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>73</v>
@@ -1807,10 +1741,10 @@
         <v>71</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>63</v>
@@ -1831,15 +1765,15 @@
         <v>34</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>49</v>
@@ -1854,10 +1788,10 @@
         <v>69</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>80</v>
@@ -1889,19 +1823,19 @@
     </row>
     <row r="15" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>85</v>
@@ -1916,13 +1850,13 @@
         <v>51</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>225</v>
+        <v>203</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>63</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
       <c r="M15" s="7" t="s">
         <v>32</v>
@@ -1942,10 +1876,10 @@
     </row>
     <row r="16" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>49</v>
@@ -1954,13 +1888,13 @@
         <v>50</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>67</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>85</v>
@@ -1969,13 +1903,13 @@
         <v>88</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>27</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
       <c r="M16" s="7" t="s">
         <v>32</v>
@@ -1996,10 +1930,10 @@
     </row>
     <row r="17" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>24</v>
@@ -2011,25 +1945,25 @@
         <v>78</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>62</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>63</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
       <c r="M17" s="7" t="s">
         <v>32</v>
@@ -2050,10 +1984,10 @@
     </row>
     <row r="18" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>46</v>
@@ -2065,19 +1999,19 @@
         <v>64</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>72</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>53</v>
@@ -2103,13 +2037,13 @@
     </row>
     <row r="19" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>66</v>
@@ -2127,7 +2061,7 @@
         <v>81</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>20</v>
@@ -2156,19 +2090,19 @@
     </row>
     <row r="20" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>41</v>
@@ -2180,16 +2114,16 @@
         <v>91</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>63</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>234</v>
+        <v>212</v>
       </c>
       <c r="M20" s="7" t="s">
         <v>32</v>
@@ -2209,16 +2143,16 @@
     </row>
     <row r="21" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>60</v>
@@ -2227,22 +2161,22 @@
         <v>26</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>60</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>27</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>234</v>
+        <v>212</v>
       </c>
       <c r="M21" s="7" t="s">
         <v>32</v>
@@ -2262,13 +2196,13 @@
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>23</v>
@@ -2277,7 +2211,7 @@
         <v>82</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>79</v>
@@ -2289,7 +2223,7 @@
         <v>18</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>63</v>
@@ -2310,18 +2244,18 @@
         <v>34</v>
       </c>
       <c r="Q22" s="7" t="s">
-        <v>234</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>67</v>
@@ -2333,19 +2267,19 @@
         <v>52</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>20</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="L23" s="7" t="s">
         <v>93</v>
@@ -2368,10 +2302,10 @@
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>52</v>
@@ -2380,13 +2314,13 @@
         <v>29</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>18</v>
@@ -2416,7 +2350,7 @@
         <v>34</v>
       </c>
       <c r="Q24" s="7" t="s">
-        <v>235</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2442,8 +2376,8 @@
   </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2499,10 +2433,10 @@
     </row>
     <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="C3" s="5">
         <v>7.09</v>
@@ -2519,10 +2453,10 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C4" s="8">
         <v>6.98</v>
@@ -2539,10 +2473,10 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="C5" s="8">
         <v>7.01</v>
@@ -2559,10 +2493,10 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="C6" s="8">
         <v>7.08</v>
@@ -2579,18 +2513,18 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="C8" s="8">
         <v>6.88</v>
@@ -2607,10 +2541,10 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="C9" s="8">
         <v>7.11</v>
@@ -2627,10 +2561,10 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="C10" s="8">
         <v>6.82</v>
@@ -2647,7 +2581,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>14</v>
@@ -2667,10 +2601,10 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="C12" s="8">
         <v>7.08</v>
@@ -2687,10 +2621,10 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="C13" s="8">
         <v>7.01</v>
@@ -2707,10 +2641,10 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="C14" s="8">
         <v>6.88</v>
@@ -2727,10 +2661,10 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="C15" s="8">
         <v>7.11</v>
@@ -2747,10 +2681,10 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="C16" s="8">
         <v>6.91</v>
@@ -2767,10 +2701,10 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="C17" s="8">
         <v>7.01</v>
@@ -2787,10 +2721,10 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="C18" s="8">
         <v>7.1</v>
@@ -2807,10 +2741,10 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="C19" s="8">
         <v>6.99</v>
@@ -2827,10 +2761,10 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="C20" s="8">
         <v>7.08</v>
@@ -2847,10 +2781,10 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="C21" s="8">
         <v>7.08</v>
@@ -2867,10 +2801,10 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="C22" s="8">
         <v>7.05</v>
@@ -2887,10 +2821,10 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="C23" s="8">
         <v>6.9</v>
@@ -2907,10 +2841,10 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="C24" s="8">
         <v>7.21</v>

</xml_diff>